<commit_message>
Refactory of file picker code
</commit_message>
<xml_diff>
--- a/demo_projects/slagbomen_project/good_DAVIE_data/slagbomen_DAVIE_data_part_1_relations.xlsx
+++ b/demo_projects/slagbomen_project/good_DAVIE_data/slagbomen_DAVIE_data_part_1_relations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\testing_output\draaiboek_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\OTLMOW-GUI\demo_projects\slagbomen_project\good_DAVIE_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8E6469-8B54-4AAD-A3E2-512BDDFF5F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2310AAF0-FAFF-4F5B-8C55-8853EF9BD467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ond#Bevestiging" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>typeURI</t>
   </si>
@@ -62,9 +62,6 @@
     <t>AWV</t>
   </si>
   <si>
-    <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Voertuiglantaarn</t>
-  </si>
-  <si>
     <t>f548e924-26b7-4062-99ca-53f4148de684-b25kZXJkZWVsI1ZvZXJ0dWlnbGFudGFhcm4</t>
   </si>
   <si>
@@ -77,27 +74,6 @@
     <t>True</t>
   </si>
   <si>
-    <t>39a02ba7-ce32-4f6d-8873-bda38d2ec23e-b25kZXJkZWVsI0JldmVzdGlnaW5n</t>
-  </si>
-  <si>
-    <t>c90adbb3-2c0d-4c74-9c8e-bccfd17d6164-b25kZXJkZWVsI1ZvZXJ0dWlnbGFudGFhcm4</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>8be72851-92c8-458c-98f3-59e4003099d7-b25kZXJkZWVsI0JldmVzdGlnaW5n</t>
-  </si>
-  <si>
-    <t>a303e80b-9863-4b47-b0c0-dadb8fc9b651-b25kZXJkZWVsI1ZvZXJ0dWlnbGFudGFhcm4</t>
-  </si>
-  <si>
-    <t>6e35a0be-7bfb-443c-b1da-6e946cc3bd2a-b25kZXJkZWVsI0JldmVzdGlnaW5n</t>
-  </si>
-  <si>
-    <t>e64e7fcb-d429-4e3d-8651-706297f14ca4-b25kZXJkZWVsI1ZvZXJ0dWlnbGFudGFhcm4</t>
-  </si>
-  <si>
     <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#HoortBij</t>
   </si>
   <si>
@@ -123,36 +99,6 @@
   </si>
   <si>
     <t>6477ff57-df59-4665-972d-368c5855f055-aW5zdGFsbGF0aWUjU2xhZ2Jvb20</t>
-  </si>
-  <si>
-    <t>2f023f87-77b3-42e2-9fbd-732d5e0bba60-b25kZXJkZWVsI0hvb3J0Qmlq</t>
-  </si>
-  <si>
-    <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Slagboomkolom</t>
-  </si>
-  <si>
-    <t>be0b7bc3-45f8-4db1-8303-ab85714c40c3-b25kZXJkZWVsI1NsYWdib29ta29sb20</t>
-  </si>
-  <si>
-    <t>e0253070-11cc-43ae-b570-1469915e9491-aW5zdGFsbGF0aWUjU2xhZ2Jvb20</t>
-  </si>
-  <si>
-    <t>7bc4d4cc-d00e-493b-bfad-9fbd9851e177-b25kZXJkZWVsI0hvb3J0Qmlq</t>
-  </si>
-  <si>
-    <t>80d1c309-54d9-49ea-8baf-032a3a15d268-b25kZXJkZWVsI0hvb3J0Qmlq</t>
-  </si>
-  <si>
-    <t>feae1d28-1c75-4a95-ac08-2fefcb777bcb-b25kZXJkZWVsI1NsYWdib29tYXJt</t>
-  </si>
-  <si>
-    <t>d74a7d43-59b3-4f56-a06a-1c9ff27da8a0-b25kZXJkZWVsI0hvb3J0Qmlq</t>
-  </si>
-  <si>
-    <t>a57fb703-7a6f-4109-b267-bbd0ee292160-b25kZXJkZWVsI1NsYWdib29ta29sb20</t>
-  </si>
-  <si>
-    <t>ea55fa42-f1a5-4898-b2cb-6de0b7f40b86-b25kZXJkZWVsI0hvb3J0Qmlq</t>
   </si>
 </sst>
 </file>
@@ -492,15 +438,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="A3:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -543,118 +489,22 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -664,13 +514,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="A4:J8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -702,228 +554,68 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
         <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>